<commit_message>
Completed the variability issue. Time to submit to Alan.
</commit_message>
<xml_diff>
--- a/comparedToTesting.xlsx
+++ b/comparedToTesting.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anupj\Documents\_WORK\Nodal Exchange Coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508F0499-CAA6-425E-95FD-3AC76FE68BCF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB62B7A5-4759-4420-8B5F-764ECA955DC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620" xr2:uid="{8D7EAA03-062D-491C-BC1E-48284A47B2D0}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="5">
   <si>
     <t>elevators</t>
   </si>
@@ -68,12 +68,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -88,9 +94,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAFEBC32-26D7-4BEC-BDD9-A0D7156BBD00}">
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,31 +426,79 @@
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="K1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="2">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>4</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="K3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="2">
+        <v>25</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -453,9 +511,33 @@
       <c r="D4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2">
+        <v>3</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2">
+        <v>2</v>
+      </c>
+      <c r="N4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <f>INT(B3*B2/B1)-1</f>
         <v>0</v>
       </c>
@@ -468,11 +550,33 @@
       <c r="D5">
         <v>969</v>
       </c>
-      <c r="L5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F5" s="3">
+        <f>INT(G3*G2/G1)-1</f>
+        <v>4</v>
+      </c>
+      <c r="G5" s="1">
+        <v>27</v>
+      </c>
+      <c r="H5" s="1">
+        <v>23</v>
+      </c>
+      <c r="I5" s="1">
+        <v>24</v>
+      </c>
+      <c r="K5" s="1">
+        <v>6</v>
+      </c>
+      <c r="L5" s="1">
+        <v>25</v>
+      </c>
+      <c r="M5" s="1">
+        <v>25</v>
+      </c>
+      <c r="N5" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>A5+1</f>
         <v>1</v>
@@ -486,11 +590,30 @@
       <c r="D6">
         <v>969</v>
       </c>
-      <c r="L6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F6" s="2">
+        <f>F5+1</f>
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="K6" s="4">
+        <f>INT(L3*L2/L1)-1</f>
+        <v>9</v>
+      </c>
+      <c r="L6" s="2">
+        <v>26</v>
+      </c>
+      <c r="M6" s="2">
+        <v>26</v>
+      </c>
+      <c r="N6" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>A6+1</f>
         <v>2</v>
@@ -504,11 +627,25 @@
       <c r="D7">
         <v>948</v>
       </c>
-      <c r="L7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="K7" s="2">
+        <f>K6+1</f>
+        <v>10</v>
+      </c>
+      <c r="L7" s="2">
+        <v>26</v>
+      </c>
+      <c r="M7" s="2">
+        <v>26</v>
+      </c>
+      <c r="N7" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f>A7+1</f>
         <v>3</v>
@@ -522,20 +659,17 @@
       <c r="D8" s="1">
         <v>907</v>
       </c>
-      <c r="L8" t="s">
-        <v>4</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <v>2</v>
-      </c>
-      <c r="O8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K8" s="2">
+        <f>K7+1</f>
+        <v>11</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -548,82 +682,153 @@
       <c r="D9">
         <v>938</v>
       </c>
-      <c r="L9" t="e">
-        <f>INT(M7*M6/M5)-1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
-      <c r="L10" t="e">
-        <f>L9+1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L11" t="e">
-        <f>L10+1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2">
+        <v>10</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>4</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
       <c r="B12">
         <v>20</v>
       </c>
-      <c r="L12" t="e">
-        <f>L11+1</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>10</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="K12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" s="2">
+        <v>20</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
       <c r="B13">
         <v>4</v>
       </c>
-      <c r="L13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>4</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="K13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2">
+        <v>2</v>
+      </c>
+      <c r="N13" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14">
         <v>10</v>
       </c>
-      <c r="L14">
+      <c r="F14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="2">
+        <v>10</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="K14" s="1">
+        <v>4</v>
+      </c>
+      <c r="L14" s="1">
+        <v>24</v>
+      </c>
+      <c r="M14" s="1">
+        <v>25</v>
+      </c>
+      <c r="N14" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>2</v>
+      </c>
+      <c r="I15" s="2">
+        <v>3</v>
+      </c>
+      <c r="K15">
         <v>5</v>
       </c>
-      <c r="M14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="L15">
+        <v>25</v>
+      </c>
+      <c r="M15">
+        <v>25</v>
+      </c>
+      <c r="N15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
         <f>INT(B14*B13/B12)-1</f>
         <v>1</v>
       </c>
@@ -636,8 +841,33 @@
       <c r="D16">
         <v>476</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" s="3">
+        <f>INT(G14*G13/G12)-1</f>
+        <v>3</v>
+      </c>
+      <c r="G16" s="1">
+        <v>29</v>
+      </c>
+      <c r="H16" s="1">
+        <v>30</v>
+      </c>
+      <c r="I16" s="1">
+        <v>30</v>
+      </c>
+      <c r="K16">
+        <v>6</v>
+      </c>
+      <c r="L16">
+        <v>26</v>
+      </c>
+      <c r="M16">
+        <v>26</v>
+      </c>
+      <c r="N16">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>A16+1</f>
         <v>2</v>
@@ -651,8 +881,30 @@
       <c r="D17">
         <v>459</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F17" s="2">
+        <f>F16+1</f>
+        <v>4</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="K17" s="4">
+        <f>INT(L12*L11/L10)-1</f>
+        <v>7</v>
+      </c>
+      <c r="L17" s="2">
+        <v>26</v>
+      </c>
+      <c r="M17" s="2">
+        <v>26</v>
+      </c>
+      <c r="N17" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f>A17+1</f>
         <v>3</v>
@@ -666,8 +918,25 @@
       <c r="D18" s="1">
         <v>447</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="K18" s="2">
+        <f>K17+1</f>
+        <v>8</v>
+      </c>
+      <c r="L18" s="2">
+        <v>25</v>
+      </c>
+      <c r="M18" s="2">
+        <v>27</v>
+      </c>
+      <c r="N18" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>A18+1</f>
         <v>4</v>
@@ -675,32 +944,93 @@
       <c r="B19" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K19" s="2">
+        <f>K18+1</f>
+        <v>9</v>
+      </c>
+      <c r="L19" s="2">
+        <v>27</v>
+      </c>
+      <c r="M19" s="2">
+        <v>28</v>
+      </c>
+      <c r="N19" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1</v>
       </c>
       <c r="B21">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2">
+        <v>10</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="K21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" s="2">
+        <v>10</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
       <c r="B22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <v>3</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="K22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2">
+        <v>4</v>
+      </c>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>2</v>
       </c>
       <c r="B23">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="2">
+        <v>10</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="K23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L23" s="2">
+        <v>15</v>
+      </c>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -713,9 +1043,33 @@
       <c r="D24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="F24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2">
+        <v>2</v>
+      </c>
+      <c r="I24" s="2">
+        <v>3</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1</v>
+      </c>
+      <c r="M24" s="2">
+        <v>2</v>
+      </c>
+      <c r="N24" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
         <f>INT(B23*B22/B21)-1</f>
         <v>1</v>
       </c>
@@ -728,8 +1082,33 @@
       <c r="D25">
         <v>242</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F25" s="3">
+        <f>INT(G23*G22/G21)-1</f>
+        <v>2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>123</v>
+      </c>
+      <c r="H25" s="1">
+        <v>123</v>
+      </c>
+      <c r="I25" s="1">
+        <v>125</v>
+      </c>
+      <c r="K25" s="1">
+        <v>3</v>
+      </c>
+      <c r="L25" s="1">
+        <v>27</v>
+      </c>
+      <c r="M25" s="1">
+        <v>27</v>
+      </c>
+      <c r="N25" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <f>A25+1</f>
         <v>2</v>
@@ -743,8 +1122,29 @@
       <c r="D26">
         <v>207</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F26" s="2">
+        <f>F25+1</f>
+        <v>3</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="K26">
+        <v>4</v>
+      </c>
+      <c r="L26">
+        <v>28</v>
+      </c>
+      <c r="M26">
+        <v>28</v>
+      </c>
+      <c r="N26">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f>A26+1</f>
         <v>3</v>
@@ -758,8 +1158,25 @@
       <c r="D27" s="1">
         <v>206</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="K27" s="4">
+        <f>INT(L23*L22/L21)-1</f>
+        <v>5</v>
+      </c>
+      <c r="L27" s="2">
+        <v>27</v>
+      </c>
+      <c r="M27" s="2">
+        <v>27</v>
+      </c>
+      <c r="N27" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>A27+1</f>
         <v>4</v>
@@ -767,32 +1184,110 @@
       <c r="B28" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K28" s="2">
+        <f>K27+1</f>
+        <v>6</v>
+      </c>
+      <c r="L28" s="2">
+        <v>27</v>
+      </c>
+      <c r="M28" s="2">
+        <v>31</v>
+      </c>
+      <c r="N28" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K29" s="2">
+        <f>K28+1</f>
+        <v>7</v>
+      </c>
+      <c r="L29" s="2">
+        <v>34</v>
+      </c>
+      <c r="M29" s="2">
+        <v>34</v>
+      </c>
+      <c r="N29" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1</v>
       </c>
       <c r="B30">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" s="2">
+        <v>10</v>
+      </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="K30" s="2">
+        <f>K29+1</f>
+        <v>8</v>
+      </c>
+      <c r="L30" s="2">
+        <v>34</v>
+      </c>
+      <c r="M30" s="2">
+        <v>36</v>
+      </c>
+      <c r="N30" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
       <c r="B31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
+        <v>2</v>
+      </c>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="K31" s="2">
+        <f>K30+1</f>
+        <v>9</v>
+      </c>
+      <c r="L31" s="2">
+        <v>34</v>
+      </c>
+      <c r="M31" s="2">
+        <v>34</v>
+      </c>
+      <c r="N31" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>
       <c r="B32">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" s="2">
+        <v>10</v>
+      </c>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -805,9 +1300,29 @@
       <c r="D33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="F33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="2">
+        <v>1</v>
+      </c>
+      <c r="H33" s="2">
+        <v>2</v>
+      </c>
+      <c r="I33" s="2">
+        <v>3</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L33" s="2">
+        <v>10</v>
+      </c>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
         <f>INT(B32*B31/B30)-1</f>
         <v>2</v>
       </c>
@@ -820,8 +1335,29 @@
       <c r="D34">
         <v>47</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F34" s="4">
+        <f>INT(G32*G31/G30)-1</f>
+        <v>1</v>
+      </c>
+      <c r="G34" s="2">
+        <v>599</v>
+      </c>
+      <c r="H34" s="2">
+        <v>599</v>
+      </c>
+      <c r="I34" s="2">
+        <v>590</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L34" s="2">
+        <v>4</v>
+      </c>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f>A34+1</f>
         <v>3</v>
@@ -835,40 +1371,138 @@
       <c r="D35" s="1">
         <v>49</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F35" s="1">
+        <f>F34+1</f>
+        <v>2</v>
+      </c>
+      <c r="G35" s="1">
+        <v>599</v>
+      </c>
+      <c r="H35" s="1">
+        <v>573</v>
+      </c>
+      <c r="I35" s="1">
+        <v>559</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L35" s="2">
+        <v>10</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F36" s="2">
+        <f>F35+1</f>
+        <v>3</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="K36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L36" s="2">
+        <v>1</v>
+      </c>
+      <c r="M36" s="2">
+        <v>2</v>
+      </c>
+      <c r="N36" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K37" s="3">
+        <f>INT(L35*L34/L33)-1</f>
+        <v>3</v>
+      </c>
+      <c r="L37" s="1">
+        <v>29</v>
+      </c>
+      <c r="M37" s="1">
+        <v>30</v>
+      </c>
+      <c r="N37" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1</v>
       </c>
       <c r="B38">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F38" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G38" s="2">
+        <v>10</v>
+      </c>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="K38" s="2">
+        <f>K37+1</f>
+        <v>4</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>0</v>
       </c>
       <c r="B39">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F39" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" s="2">
+        <v>1</v>
+      </c>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>2</v>
       </c>
       <c r="B40">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G40" s="2">
+        <v>10</v>
+      </c>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="K40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L40" s="2">
+        <v>10</v>
+      </c>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -881,9 +1515,29 @@
       <c r="D41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+      <c r="F41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G41" s="2">
+        <v>1</v>
+      </c>
+      <c r="H41" s="2">
+        <v>2</v>
+      </c>
+      <c r="I41" s="2">
+        <v>3</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L41" s="2">
+        <v>4</v>
+      </c>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
         <f>INT(B40*B39/B38)-1</f>
         <v>3</v>
       </c>
@@ -896,8 +1550,29 @@
       <c r="D42" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F42" s="4">
+        <f>INT(G40*G39/G38)-1</f>
+        <v>0</v>
+      </c>
+      <c r="G42" s="2">
+        <v>2170</v>
+      </c>
+      <c r="H42" s="2">
+        <v>2187</v>
+      </c>
+      <c r="I42" s="2">
+        <v>2196</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L42" s="2">
+        <v>5</v>
+      </c>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <f>A42+1</f>
         <v>4</v>
@@ -905,6 +1580,95 @@
       <c r="B43" t="s">
         <v>3</v>
       </c>
+      <c r="F43" s="1">
+        <f>F42+1</f>
+        <v>1</v>
+      </c>
+      <c r="G43" s="1">
+        <v>2170</v>
+      </c>
+      <c r="H43" s="1">
+        <v>2170</v>
+      </c>
+      <c r="I43" s="1">
+        <v>2196</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L43" s="2">
+        <v>1</v>
+      </c>
+      <c r="M43" s="2">
+        <v>2</v>
+      </c>
+      <c r="N43" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F44" s="2">
+        <f>F43+1</f>
+        <v>2</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="K44" s="3">
+        <f>INT(L42*L41/L40)-1</f>
+        <v>1</v>
+      </c>
+      <c r="L44" s="1">
+        <v>372</v>
+      </c>
+      <c r="M44" s="1">
+        <v>378</v>
+      </c>
+      <c r="N44" s="1">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="K45" s="2">
+        <f>K44+1</f>
+        <v>2</v>
+      </c>
+      <c r="L45" s="2">
+        <v>364</v>
+      </c>
+      <c r="M45" s="2">
+        <v>970</v>
+      </c>
+      <c r="N45" s="2">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="K46" s="2">
+        <f>K45+1</f>
+        <v>3</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>